<commit_message>
AGU 2021 Code Version
This is the version of the codes in this repo that was used to produce the 2021 AGU poster "Observations of Jupiter in the 645nm Ammonia Absorption Band"
</commit_message>
<xml_diff>
--- a/MoonsColorSlopeFromLiterature.xlsx
+++ b/MoonsColorSlopeFromLiterature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F269490F-9C54-4B36-B934-3CFF0E7BD8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0558837-43FE-4A91-A129-D6E099C1BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="-110" windowWidth="17990" windowHeight="11020" activeTab="4" xr2:uid="{CD1319F5-58B1-4D86-AAAC-92CA0B7E9033}"/>
   </bookViews>
@@ -2790,7 +2790,7 @@
   <dimension ref="B1:G125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10456,7 +10456,7 @@
   <dimension ref="B1:L147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>